<commit_message>
Clarify headings and add note that gain is not considered.
</commit_message>
<xml_diff>
--- a/LDMP/data/summary_table_tc.xlsx
+++ b/LDMP/data/summary_table_tc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B074C28B-E63B-41BB-B693-8AD05E5E51A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A95545-62CA-4AA5-81E5-FC3EB499E0C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17070" yWindow="1980" windowWidth="19200" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="8355" windowWidth="19410" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Carbon Summary Table" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>The boundaries, names, and designations used in this report do not imply official endorsement or acceptance by Conservation International Foundation, or its partner organizations and contributors.  This report is available under the terms of Creative Commons Attribution 4.0 International License (CC BY 4.0).</t>
   </si>
@@ -38,16 +38,10 @@
     <t>For more information on Trends.Earth, see http://trends.earth, or contact the team at trends.earth@conservation.org.</t>
   </si>
   <si>
-    <t>Trends.Earth carbon change summary table</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
     <t>Analysis notes:</t>
-  </si>
-  <si>
-    <t>Summary of carbon change</t>
   </si>
   <si>
     <t>Area (hectares)</t>
@@ -120,9 +114,6 @@
     <t>Final year:</t>
   </si>
   <si>
-    <t>Carbon change from baseline to final year</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -151,6 +142,18 @@
   </si>
   <si>
     <t>Land cover change summary</t>
+  </si>
+  <si>
+    <t>Trends.Earth carbon loss due to deforestation summary table</t>
+  </si>
+  <si>
+    <t>*Due to limitations in the underlying datasets, potential gains of carbon are not captured in this analysis. This analysis considers only carbon loss due to deforestation, without considering any potential gains due to increased tree cover.</t>
+  </si>
+  <si>
+    <t>Summary of carbon loss due to deforestation*</t>
+  </si>
+  <si>
+    <t>Carbon loss by year*</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -436,6 +439,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,8 +468,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -798,7 +813,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -814,7 +829,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -826,45 +841,45 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="A3" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
+      <c r="A6" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
     </row>
     <row r="7" spans="1:6" s="16" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="34" t="str">
@@ -876,7 +891,7 @@
     <row r="9" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="34" t="str">
@@ -888,7 +903,7 @@
     <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="34" t="str">
@@ -900,7 +915,7 @@
     <row r="11" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34" t="str">
@@ -912,7 +927,7 @@
     <row r="12" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="32">
         <f>SUM(C8:C11)</f>
@@ -932,20 +947,20 @@
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:6" s="44" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
+      <c r="A14" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="42"/>
       <c r="E15" s="10"/>
@@ -954,17 +969,17 @@
       <c r="A16" s="9"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="50"/>
+      <c r="B17" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="51"/>
       <c r="D17" s="36">
         <f>SUM(B24:B44)</f>
         <v>0</v>
@@ -974,10 +989,10 @@
     </row>
     <row r="18" spans="1:8" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
-      <c r="B18" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="54"/>
+      <c r="B18" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="55"/>
       <c r="D18" s="36">
         <f>SUM(D24:D44)</f>
         <v>0</v>
@@ -986,10 +1001,10 @@
     </row>
     <row r="19" spans="1:8" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
-      <c r="B19" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="50"/>
+      <c r="B19" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="51"/>
       <c r="D19" s="36">
         <f>SUM(F24:F44)</f>
         <v>0</v>
@@ -1000,14 +1015,14 @@
       <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
+      <c r="A21" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -1019,22 +1034,22 @@
     </row>
     <row r="23" spans="1:8" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>13</v>
-      </c>
       <c r="E23" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="25" t="s">
         <v>12</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1044,7 +1059,7 @@
         <f>C8-B24</f>
         <v>0</v>
       </c>
-      <c r="D24" s="56"/>
+      <c r="D24" s="46"/>
       <c r="E24" s="30">
         <f>E8-D24</f>
         <v>0</v>
@@ -1062,7 +1077,7 @@
         <f>IF(ISBLANK(B25),"",C24-B25)</f>
         <v/>
       </c>
-      <c r="D25" s="56"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="30" t="str">
         <f>IF(ISBLANK(D25),"",E24-D25)</f>
         <v/>
@@ -1080,7 +1095,7 @@
         <f t="shared" ref="C26:C44" si="1">IF(ISBLANK(B26),"",C25-B26)</f>
         <v/>
       </c>
-      <c r="D26" s="56"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="30" t="str">
         <f t="shared" ref="E26:E44" si="2">IF(ISBLANK(D26),"",E25-D26)</f>
         <v/>
@@ -1099,7 +1114,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1117,7 +1132,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D28" s="56"/>
+      <c r="D28" s="46"/>
       <c r="E28" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1135,7 +1150,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D29" s="56"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1153,7 +1168,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D30" s="56"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1171,7 +1186,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D31" s="56"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1189,7 +1204,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D32" s="56"/>
+      <c r="D32" s="46"/>
       <c r="E32" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1207,7 +1222,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D33" s="56"/>
+      <c r="D33" s="46"/>
       <c r="E33" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1225,7 +1240,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D34" s="56"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1243,7 +1258,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D35" s="56"/>
+      <c r="D35" s="46"/>
       <c r="E35" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1261,7 +1276,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D36" s="56"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1279,7 +1294,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D37" s="56"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1297,7 +1312,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D38" s="56"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1315,7 +1330,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D39" s="56"/>
+      <c r="D39" s="46"/>
       <c r="E39" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1333,7 +1348,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D40" s="56"/>
+      <c r="D40" s="46"/>
       <c r="E40" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1351,7 +1366,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D41" s="56"/>
+      <c r="D41" s="46"/>
       <c r="E41" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1369,7 +1384,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D42" s="56"/>
+      <c r="D42" s="46"/>
       <c r="E42" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1387,7 +1402,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D43" s="56"/>
+      <c r="D43" s="46"/>
       <c r="E43" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1405,7 +1420,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D44" s="56"/>
+      <c r="D44" s="46"/>
       <c r="E44" s="30" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1416,73 +1431,93 @@
       </c>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
+    <row r="45" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-    </row>
-    <row r="47" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-    </row>
-    <row r="48" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:6" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="48" t="s">
+    <row r="46" spans="1:8" s="13" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="H47" s="15"/>
+    </row>
+    <row r="48" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+    </row>
+    <row r="49" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+    </row>
+    <row r="50" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:6" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="48" t="s">
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="B46:F47"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="B48:F49"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A51:F51"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A46:F46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>

</xml_diff>